<commit_message>
docs(Ver. 0.6.0.0 - beta): 🛠 Stocket - Docs
Se ha añadido documentación de bitacora y se ha corregido contraseña de correo electrónico
</commit_message>
<xml_diff>
--- a/docs/GFPI-F-147_Formato_bitácora_etapa_productiva - V2.xlsx
+++ b/docs/GFPI-F-147_Formato_bitácora_etapa_productiva - V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\PycharmProjects\Stocket\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86259429-E937-47DD-BDA9-7A7FCE7E850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562B67B5-314F-487C-A556-B77EB8901DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,23 +417,6 @@
     <t>ANALISIS Y DESARROLLO DE SISTEMAS DE INFORMACIÓN</t>
   </si>
   <si>
-    <t>4-SEPTIEMBRE-2023 AL 18-SEPTIEMBRE-2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Ver. 0.5.0.0 - alpha"
-- Gestion de mantenimientos: se ha finalizado el desarrollo de modulo de mantenimientos, ahora el sistema puede crear, finalizar historias de mantenimientos y se puede alterar el estado de los elementos para iniciar procesos de baja
-- Gestion de bajas: se ha creado modulo de bajas, ahora se crean reportes sobre los elementos que serán borrados y se muestra informacion sobre su fecha de borrado del sistema.
-- Reportes del sistema: Ahora se ha creado un apartado en el sistema que muestra los elementos cuyas historias de mantenimiento se encuentran abiertas y elementos cuya baja se encuentra en proceso.
-"Ver. 0.6.0.0 - beta"
-- Se ha finalizado el proceso de desarrollo del sistema, en vista de que se han construido todos los modulos definidos
-- Se ha creado reporte de fallos en el archivo bugs.md
-- Se han realizado mejoras de codigo y optimizacion del mismo para corregir errores identificados
-- Se ha desplegado el producto para su testeo en fase beta, se encuentra disponible en la red para su uso
-- Se continua con la corrección de errores y mejoras	
-- Todas las funciones de autenticacion y registros fueron optimizadas, ahora el sistema permite crear usuarios y se requiere un correo válido para realizar operaciones.					
-								</t>
-  </si>
-  <si>
     <t xml:space="preserve">Historial de cambios en repositorio GitHub https://github.com/luchompi/Stocket
 Repositorio GitHub de despliegue para pruebas en https://github.com/luchompi/stocket-deploy
 URL para testeo en https://stocket-deploy.vercel.app/
@@ -444,6 +427,16 @@
   </si>
   <si>
     <t>NINGUNA</t>
+  </si>
+  <si>
+    <t>19-SEPTIEMBRE-2023 - 03-OCTUBRE-2023</t>
+  </si>
+  <si>
+    <t>"Ver. 0.6.42.0 - beta"
+- Se ha creado archivo de reporte con errores comunes bajo el nombre bugs.md
+- Se han corregido errores identificados el reporte de bugs.md
+- Se ha empezado a escribir manuales de uso
+- Se ha alterado contraseña de correo electronico configurado para autenticación</t>
   </si>
 </sst>
 </file>
@@ -991,81 +984,135 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1091,33 +1138,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1270,33 +1290,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1829,8 +1822,8 @@
   </sheetPr>
   <dimension ref="B1:Y56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:J30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1856,14 +1849,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="72"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
@@ -1876,22 +1869,22 @@
       <c r="S1" s="29"/>
       <c r="T1" s="29"/>
       <c r="U1" s="29"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="69" t="s">
+      <c r="V1" s="83"/>
+      <c r="W1" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
     </row>
     <row r="2" spans="2:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
@@ -1904,25 +1897,25 @@
       <c r="S2" s="29"/>
       <c r="T2" s="29"/>
       <c r="U2" s="29"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="71" t="s">
+      <c r="V2" s="83"/>
+      <c r="W2" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
     </row>
     <row r="3" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
@@ -1940,17 +1933,17 @@
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
@@ -1968,114 +1961,114 @@
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="2:25" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="60"/>
-      <c r="W5" s="60"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="61"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="69"/>
     </row>
     <row r="6" spans="2:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="61"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="69"/>
     </row>
     <row r="7" spans="2:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="62"/>
-      <c r="Y7" s="62"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="70"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="70"/>
     </row>
     <row r="8" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="63"/>
-      <c r="U8" s="63"/>
-      <c r="V8" s="63"/>
-      <c r="W8" s="63"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="63"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
     </row>
     <row r="9" spans="2:25" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="35" t="s">
@@ -2094,14 +2087,14 @@
       <c r="M9" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
       <c r="P9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="92"/>
-      <c r="R9" s="92"/>
-      <c r="S9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="94"/>
       <c r="T9" s="35" t="s">
         <v>3</v>
       </c>
@@ -2112,36 +2105,36 @@
       <c r="Y9" s="35"/>
     </row>
     <row r="10" spans="2:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="81"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="99"/>
       <c r="M10" s="35"/>
-      <c r="N10" s="94"/>
-      <c r="O10" s="94"/>
+      <c r="N10" s="95"/>
+      <c r="O10" s="95"/>
       <c r="P10" s="89">
-        <v>7</v>
-      </c>
-      <c r="Q10" s="92"/>
-      <c r="R10" s="92"/>
-      <c r="S10" s="93"/>
-      <c r="T10" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="U10" s="71"/>
-      <c r="V10" s="71"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="71"/>
-      <c r="Y10" s="71"/>
+        <v>8</v>
+      </c>
+      <c r="Q10" s="93"/>
+      <c r="R10" s="93"/>
+      <c r="S10" s="94"/>
+      <c r="T10" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="U10" s="78"/>
+      <c r="V10" s="78"/>
+      <c r="W10" s="78"/>
+      <c r="X10" s="78"/>
+      <c r="Y10" s="78"/>
     </row>
     <row r="11" spans="2:25" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
@@ -2170,49 +2163,49 @@
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="2:25" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="73" t="s">
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73" t="s">
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="73"/>
-      <c r="S12" s="73"/>
-      <c r="T12" s="73"/>
-      <c r="U12" s="73"/>
-      <c r="V12" s="73"/>
-      <c r="W12" s="73"/>
-      <c r="X12" s="73"/>
-      <c r="Y12" s="73"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="82"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="82"/>
+      <c r="X12" s="82"/>
+      <c r="Y12" s="82"/>
     </row>
     <row r="13" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="100" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="84"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="102"/>
       <c r="K13" s="47" t="s">
         <v>115</v>
       </c>
@@ -2221,7 +2214,7 @@
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
       <c r="P13" s="47"/>
-      <c r="Q13" s="78" t="s">
+      <c r="Q13" s="96" t="s">
         <v>116</v>
       </c>
       <c r="R13" s="47"/>
@@ -2260,32 +2253,32 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="64"/>
-      <c r="X15" s="64"/>
-      <c r="Y15" s="64"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="72"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="72"/>
+      <c r="W15" s="72"/>
+      <c r="X15" s="72"/>
+      <c r="Y15" s="72"/>
     </row>
     <row r="16" spans="2:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="37" t="s">
@@ -2426,7 +2419,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
       <c r="I20" s="48"/>
-      <c r="J20" s="68">
+      <c r="J20" s="76">
         <v>1118855506</v>
       </c>
       <c r="K20" s="48"/>
@@ -2506,34 +2499,34 @@
       <c r="Y22" s="36"/>
     </row>
     <row r="23" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="65">
+      <c r="B23" s="73">
         <v>2281590</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="65" t="s">
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="66"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="66"/>
-      <c r="S23" s="66"/>
-      <c r="T23" s="66"/>
-      <c r="U23" s="66"/>
-      <c r="V23" s="66"/>
-      <c r="W23" s="66"/>
-      <c r="X23" s="66"/>
-      <c r="Y23" s="67"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="75"/>
     </row>
     <row r="24" spans="2:25" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -2598,172 +2591,172 @@
       <c r="Y25" s="91"/>
     </row>
     <row r="26" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="146" t="s">
+      <c r="B26" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="52">
+        <v>45188</v>
+      </c>
+      <c r="L26" s="53"/>
+      <c r="M26" s="52">
+        <v>45202</v>
+      </c>
+      <c r="N26" s="53"/>
+      <c r="O26" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="147"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
-      <c r="F26" s="147"/>
-      <c r="G26" s="147"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="147"/>
-      <c r="J26" s="148"/>
-      <c r="K26" s="53">
-        <v>45173</v>
-      </c>
-      <c r="L26" s="54"/>
-      <c r="M26" s="53">
-        <v>45187</v>
-      </c>
-      <c r="N26" s="54"/>
-      <c r="O26" s="146" t="s">
-        <v>123</v>
-      </c>
-      <c r="P26" s="147"/>
-      <c r="Q26" s="147"/>
-      <c r="R26" s="147"/>
-      <c r="S26" s="147"/>
-      <c r="T26" s="148"/>
-      <c r="U26" s="146" t="s">
-        <v>124</v>
-      </c>
-      <c r="V26" s="147"/>
-      <c r="W26" s="147"/>
-      <c r="X26" s="147"/>
-      <c r="Y26" s="148"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="59"/>
+      <c r="Y26" s="60"/>
     </row>
     <row r="27" spans="2:25" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="149"/>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="151"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="149"/>
-      <c r="P27" s="150"/>
-      <c r="Q27" s="150"/>
-      <c r="R27" s="150"/>
-      <c r="S27" s="150"/>
-      <c r="T27" s="151"/>
-      <c r="U27" s="149"/>
-      <c r="V27" s="150"/>
-      <c r="W27" s="150"/>
-      <c r="X27" s="150"/>
-      <c r="Y27" s="151"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="63"/>
     </row>
     <row r="28" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="149"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
-      <c r="H28" s="150"/>
-      <c r="I28" s="150"/>
-      <c r="J28" s="151"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="149"/>
-      <c r="P28" s="150"/>
-      <c r="Q28" s="150"/>
-      <c r="R28" s="150"/>
-      <c r="S28" s="150"/>
-      <c r="T28" s="151"/>
-      <c r="U28" s="149"/>
-      <c r="V28" s="150"/>
-      <c r="W28" s="150"/>
-      <c r="X28" s="150"/>
-      <c r="Y28" s="151"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="62"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="61"/>
+      <c r="V28" s="62"/>
+      <c r="W28" s="62"/>
+      <c r="X28" s="62"/>
+      <c r="Y28" s="63"/>
     </row>
     <row r="29" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="149"/>
-      <c r="C29" s="150"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
-      <c r="G29" s="150"/>
-      <c r="H29" s="150"/>
-      <c r="I29" s="150"/>
-      <c r="J29" s="151"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="149"/>
-      <c r="P29" s="150"/>
-      <c r="Q29" s="150"/>
-      <c r="R29" s="150"/>
-      <c r="S29" s="150"/>
-      <c r="T29" s="151"/>
-      <c r="U29" s="149"/>
-      <c r="V29" s="150"/>
-      <c r="W29" s="150"/>
-      <c r="X29" s="150"/>
-      <c r="Y29" s="151"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="62"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="61"/>
+      <c r="V29" s="62"/>
+      <c r="W29" s="62"/>
+      <c r="X29" s="62"/>
+      <c r="Y29" s="63"/>
     </row>
     <row r="30" spans="2:25" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="153"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="153"/>
-      <c r="H30" s="153"/>
-      <c r="I30" s="153"/>
-      <c r="J30" s="154"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="152"/>
-      <c r="P30" s="153"/>
-      <c r="Q30" s="153"/>
-      <c r="R30" s="153"/>
-      <c r="S30" s="153"/>
-      <c r="T30" s="154"/>
-      <c r="U30" s="152"/>
-      <c r="V30" s="153"/>
-      <c r="W30" s="153"/>
-      <c r="X30" s="153"/>
-      <c r="Y30" s="154"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="65"/>
+      <c r="X30" s="65"/>
+      <c r="Y30" s="66"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="52"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="92"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="92"/>
+      <c r="Q31" s="92"/>
+      <c r="R31" s="92"/>
+      <c r="S31" s="92"/>
+      <c r="T31" s="92"/>
+      <c r="U31" s="92"/>
+      <c r="V31" s="92"/>
+      <c r="W31" s="92"/>
+      <c r="X31" s="92"/>
+      <c r="Y31" s="92"/>
     </row>
     <row r="32" spans="2:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -3124,6 +3117,13 @@
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="M10:O10"/>
     <mergeCell ref="M26:N30"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
     <mergeCell ref="B16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="B42:I42"/>
@@ -3138,13 +3138,8 @@
     <mergeCell ref="B25:J25"/>
     <mergeCell ref="O25:T25"/>
     <mergeCell ref="U25:Y25"/>
-    <mergeCell ref="Q12:Y12"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:Y13"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="T38:X38"/>
+    <mergeCell ref="B31:Y31"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="B1:V2"/>
@@ -3166,8 +3161,6 @@
     <mergeCell ref="T9:Y9"/>
     <mergeCell ref="T10:Y10"/>
     <mergeCell ref="B9:L9"/>
-    <mergeCell ref="T38:X38"/>
-    <mergeCell ref="B31:Y31"/>
     <mergeCell ref="B38:I38"/>
     <mergeCell ref="K26:L30"/>
     <mergeCell ref="O26:T30"/>
@@ -3226,47 +3219,47 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
     <row r="3" spans="2:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
     <row r="4" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="122" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="122"/>
       <c r="K4" s="27" t="s">
         <v>109</v>
       </c>
@@ -3275,15 +3268,15 @@
       <c r="N4" s="18"/>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
       <c r="K5" s="28" t="s">
         <v>87</v>
       </c>
@@ -3293,277 +3286,277 @@
       <c r="O5" s="18"/>
     </row>
     <row r="6" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
     </row>
     <row r="7" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
     </row>
     <row r="8" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="108"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="102"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
+      <c r="K10" s="111"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="102"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="111"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="102"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="111"/>
     </row>
     <row r="13" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="102"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="111"/>
     </row>
     <row r="14" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="102"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="111"/>
     </row>
     <row r="15" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="101"/>
-      <c r="K15" s="102"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="111"/>
     </row>
     <row r="16" spans="2:15" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="102"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="111"/>
     </row>
     <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="101"/>
-      <c r="J17" s="101"/>
-      <c r="K17" s="102"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="111"/>
     </row>
     <row r="18" spans="2:12" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="102"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="111"/>
     </row>
     <row r="19" spans="2:12" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="100"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="101"/>
-      <c r="J19" s="101"/>
-      <c r="K19" s="102"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="111"/>
     </row>
     <row r="20" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="100"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="101"/>
-      <c r="K20" s="102"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="111"/>
     </row>
     <row r="21" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="103"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="105"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="114"/>
     </row>
     <row r="22" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
-      <c r="K22" s="109"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
     </row>
     <row r="23" spans="2:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="110"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
     </row>
     <row r="24" spans="2:12" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="111" t="s">
+      <c r="C24" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111" t="s">
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
       <c r="L24" s="20"/>
     </row>
     <row r="25" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="107"/>
-      <c r="K25" s="108"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="117"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="116"/>
+      <c r="J25" s="116"/>
+      <c r="K25" s="117"/>
     </row>
     <row r="26" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="114"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="115"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="124"/>
       <c r="H26" s="24"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
@@ -3573,391 +3566,391 @@
       <c r="B27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="104"/>
     </row>
     <row r="28" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="108"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
     </row>
     <row r="29" spans="2:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="95" t="s">
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="104"/>
     </row>
     <row r="30" spans="2:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95" t="s">
+      <c r="D30" s="104"/>
+      <c r="E30" s="104"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
     </row>
     <row r="31" spans="2:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="95" t="s">
+      <c r="C31" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95" t="s">
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
     </row>
     <row r="32" spans="2:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="95"/>
+      <c r="D32" s="104"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="95" t="s">
+      <c r="C33" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
     </row>
     <row r="34" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="95" t="s">
+      <c r="C34" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="95"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="104"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="104"/>
     </row>
     <row r="36" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="95" t="s">
+      <c r="C36" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95" t="s">
+      <c r="D36" s="104"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="104"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="I36" s="95"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="95"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="104"/>
     </row>
     <row r="37" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="95" t="s">
+      <c r="C37" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="95"/>
+      <c r="D37" s="104"/>
+      <c r="E37" s="104"/>
+      <c r="F37" s="104"/>
+      <c r="G37" s="104"/>
+      <c r="H37" s="104"/>
+      <c r="I37" s="104"/>
+      <c r="J37" s="104"/>
+      <c r="K37" s="104"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="95"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="95"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="95"/>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104"/>
+      <c r="J38" s="104"/>
+      <c r="K38" s="104"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="95" t="s">
+      <c r="C39" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="104"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="104"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="104"/>
+      <c r="J39" s="104"/>
+      <c r="K39" s="104"/>
     </row>
     <row r="40" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="95"/>
-      <c r="G40" s="95"/>
-      <c r="H40" s="95"/>
-      <c r="I40" s="95"/>
-      <c r="J40" s="95"/>
-      <c r="K40" s="95"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
     </row>
     <row r="41" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="95" t="s">
+      <c r="C41" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="95"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="95"/>
-      <c r="G41" s="95"/>
-      <c r="H41" s="95"/>
-      <c r="I41" s="95"/>
-      <c r="J41" s="95"/>
-      <c r="K41" s="95"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="104"/>
+      <c r="J41" s="104"/>
+      <c r="K41" s="104"/>
     </row>
     <row r="42" spans="2:11" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="95" t="s">
+      <c r="C42" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95" t="s">
+      <c r="D42" s="104"/>
+      <c r="E42" s="104"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="95"/>
+      <c r="I42" s="104"/>
+      <c r="J42" s="104"/>
+      <c r="K42" s="104"/>
     </row>
     <row r="43" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="95"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="95"/>
-      <c r="J43" s="95"/>
-      <c r="K43" s="95"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="104"/>
+      <c r="J43" s="104"/>
+      <c r="K43" s="104"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="106" t="s">
+      <c r="C44" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="107"/>
-      <c r="E44" s="107"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="108"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="107"/>
-      <c r="J44" s="107"/>
-      <c r="K44" s="108"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="116"/>
+      <c r="G44" s="117"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="116"/>
+      <c r="J44" s="116"/>
+      <c r="K44" s="117"/>
     </row>
     <row r="45" spans="2:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="95" t="s">
+      <c r="C45" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="95"/>
-      <c r="E45" s="95"/>
-      <c r="F45" s="95"/>
-      <c r="G45" s="95"/>
-      <c r="H45" s="95"/>
-      <c r="I45" s="95"/>
-      <c r="J45" s="95"/>
-      <c r="K45" s="95"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="104"/>
+      <c r="F45" s="104"/>
+      <c r="G45" s="104"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="104"/>
+      <c r="K45" s="104"/>
     </row>
     <row r="46" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="95" t="s">
+      <c r="C46" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="D46" s="95"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="95"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="95"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="104"/>
+      <c r="G46" s="104"/>
+      <c r="H46" s="104"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="104"/>
+      <c r="K46" s="104"/>
     </row>
     <row r="47" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="106" t="s">
+      <c r="C47" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="107"/>
-      <c r="E47" s="107"/>
-      <c r="F47" s="107"/>
-      <c r="G47" s="108"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="107"/>
-      <c r="J47" s="107"/>
-      <c r="K47" s="108"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="117"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="116"/>
+      <c r="J47" s="116"/>
+      <c r="K47" s="117"/>
     </row>
     <row r="48" spans="2:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="95" t="s">
+      <c r="C48" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="104"/>
+      <c r="G48" s="104"/>
+      <c r="H48" s="104"/>
+      <c r="I48" s="104"/>
+      <c r="J48" s="104"/>
+      <c r="K48" s="104"/>
     </row>
     <row r="49" spans="2:11" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="95" t="s">
+      <c r="C49" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="95"/>
-      <c r="E49" s="95"/>
-      <c r="F49" s="95"/>
-      <c r="G49" s="95"/>
-      <c r="H49" s="95"/>
-      <c r="I49" s="95"/>
-      <c r="J49" s="95"/>
-      <c r="K49" s="95"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="104"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="104"/>
+      <c r="H49" s="104"/>
+      <c r="I49" s="104"/>
+      <c r="J49" s="104"/>
+      <c r="K49" s="104"/>
     </row>
     <row r="50" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="96"/>
-      <c r="C50" s="96"/>
-      <c r="D50" s="96"/>
-      <c r="E50" s="96"/>
-      <c r="F50" s="96"/>
-      <c r="G50" s="96"/>
-      <c r="H50" s="96"/>
-      <c r="I50" s="96"/>
-      <c r="J50" s="96"/>
-      <c r="K50" s="96"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="105"/>
+      <c r="D50" s="105"/>
+      <c r="E50" s="105"/>
+      <c r="F50" s="105"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="105"/>
+      <c r="I50" s="105"/>
+      <c r="J50" s="105"/>
+      <c r="K50" s="105"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="8"/>
@@ -4068,124 +4061,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="116" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="125"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="116"/>
-      <c r="W1" s="116"/>
-      <c r="X1" s="116"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125"/>
+      <c r="X1" s="125"/>
     </row>
     <row r="2" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="124" t="s">
+      <c r="A2" s="125"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
+      <c r="V2" s="133"/>
+      <c r="W2" s="133"/>
+      <c r="X2" s="133"/>
     </row>
     <row r="3" spans="1:24" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U3" s="125"/>
-      <c r="V3" s="125"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="125"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="121" t="s">
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
-      <c r="W4" s="122"/>
-      <c r="X4" s="123"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="132"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="118"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="119"/>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
-      <c r="W5" s="119"/>
-      <c r="X5" s="120"/>
+      <c r="A5" s="127"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="128"/>
+      <c r="P5" s="128"/>
+      <c r="Q5" s="128"/>
+      <c r="R5" s="128"/>
+      <c r="S5" s="128"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="129"/>
     </row>
     <row r="6" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -4214,36 +4207,36 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117" t="s">
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117" t="s">
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="126"/>
+      <c r="T7" s="126"/>
+      <c r="U7" s="126"/>
+      <c r="V7" s="126"/>
+      <c r="W7" s="126"/>
+      <c r="X7" s="126"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48"/>
@@ -4255,25 +4248,25 @@
       <c r="G8" s="48"/>
       <c r="H8" s="48"/>
       <c r="I8" s="48"/>
-      <c r="J8" s="126" t="s">
+      <c r="J8" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="126" t="s">
+      <c r="K8" s="136"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="136"/>
+      <c r="N8" s="136"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="127"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="128"/>
+      <c r="Q8" s="136"/>
+      <c r="R8" s="136"/>
+      <c r="S8" s="136"/>
+      <c r="T8" s="136"/>
+      <c r="U8" s="136"/>
+      <c r="V8" s="136"/>
+      <c r="W8" s="136"/>
+      <c r="X8" s="137"/>
     </row>
     <row r="9" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -4302,32 +4295,32 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="72"/>
+      <c r="X10" s="72"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
@@ -4390,36 +4383,36 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
-      <c r="J13" s="117" t="s">
+      <c r="B13" s="126"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117" t="s">
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="126"/>
+      <c r="O13" s="126"/>
+      <c r="P13" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="117"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
+      <c r="Q13" s="126"/>
+      <c r="R13" s="126"/>
+      <c r="S13" s="126"/>
+      <c r="T13" s="126"/>
+      <c r="U13" s="126"/>
+      <c r="V13" s="126"/>
+      <c r="W13" s="126"/>
+      <c r="X13" s="126"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
@@ -4431,25 +4424,25 @@
       <c r="G14" s="48"/>
       <c r="H14" s="48"/>
       <c r="I14" s="48"/>
-      <c r="J14" s="126" t="s">
+      <c r="J14" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="127"/>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
-      <c r="N14" s="127"/>
-      <c r="O14" s="128"/>
-      <c r="P14" s="126" t="s">
+      <c r="K14" s="136"/>
+      <c r="L14" s="136"/>
+      <c r="M14" s="136"/>
+      <c r="N14" s="136"/>
+      <c r="O14" s="137"/>
+      <c r="P14" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="127"/>
-      <c r="R14" s="127"/>
-      <c r="S14" s="127"/>
-      <c r="T14" s="127"/>
-      <c r="U14" s="127"/>
-      <c r="V14" s="127"/>
-      <c r="W14" s="127"/>
-      <c r="X14" s="128"/>
+      <c r="Q14" s="136"/>
+      <c r="R14" s="136"/>
+      <c r="S14" s="136"/>
+      <c r="T14" s="136"/>
+      <c r="U14" s="136"/>
+      <c r="V14" s="136"/>
+      <c r="W14" s="136"/>
+      <c r="X14" s="137"/>
     </row>
     <row r="15" spans="1:24" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -4489,12 +4482,12 @@
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
-      <c r="J16" s="134" t="s">
+      <c r="J16" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="134"/>
-      <c r="L16" s="134"/>
-      <c r="M16" s="134"/>
+      <c r="K16" s="143"/>
+      <c r="L16" s="143"/>
+      <c r="M16" s="143"/>
       <c r="N16" s="31" t="s">
         <v>13</v>
       </c>
@@ -4503,137 +4496,137 @@
       <c r="Q16" s="31"/>
       <c r="R16" s="31"/>
       <c r="S16" s="31"/>
-      <c r="T16" s="135" t="s">
+      <c r="T16" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="135"/>
-      <c r="V16" s="135"/>
-      <c r="W16" s="135"/>
-      <c r="X16" s="135"/>
+      <c r="U16" s="144"/>
+      <c r="V16" s="144"/>
+      <c r="W16" s="144"/>
+      <c r="X16" s="144"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="129" t="s">
+      <c r="A17" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="124"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="124"/>
-      <c r="H17" s="124"/>
-      <c r="I17" s="130"/>
-      <c r="J17" s="136" t="s">
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="145" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
-      <c r="M17" s="138"/>
-      <c r="N17" s="129" t="s">
+      <c r="K17" s="146"/>
+      <c r="L17" s="146"/>
+      <c r="M17" s="147"/>
+      <c r="N17" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
-      <c r="R17" s="124"/>
-      <c r="S17" s="130"/>
-      <c r="T17" s="129" t="s">
+      <c r="O17" s="133"/>
+      <c r="P17" s="133"/>
+      <c r="Q17" s="133"/>
+      <c r="R17" s="133"/>
+      <c r="S17" s="139"/>
+      <c r="T17" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="U17" s="124"/>
-      <c r="V17" s="124"/>
-      <c r="W17" s="124"/>
-      <c r="X17" s="130"/>
+      <c r="U17" s="133"/>
+      <c r="V17" s="133"/>
+      <c r="W17" s="133"/>
+      <c r="X17" s="139"/>
     </row>
     <row r="18" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="131"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="133"/>
-      <c r="J18" s="139"/>
-      <c r="K18" s="140"/>
-      <c r="L18" s="140"/>
-      <c r="M18" s="141"/>
-      <c r="N18" s="131"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="132"/>
-      <c r="Q18" s="132"/>
-      <c r="R18" s="132"/>
-      <c r="S18" s="133"/>
-      <c r="T18" s="131"/>
-      <c r="U18" s="132"/>
-      <c r="V18" s="132"/>
-      <c r="W18" s="132"/>
-      <c r="X18" s="133"/>
+      <c r="A18" s="140"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="148"/>
+      <c r="K18" s="149"/>
+      <c r="L18" s="149"/>
+      <c r="M18" s="150"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="141"/>
+      <c r="P18" s="141"/>
+      <c r="Q18" s="141"/>
+      <c r="R18" s="141"/>
+      <c r="S18" s="142"/>
+      <c r="T18" s="140"/>
+      <c r="U18" s="141"/>
+      <c r="V18" s="141"/>
+      <c r="W18" s="141"/>
+      <c r="X18" s="142"/>
     </row>
     <row r="19" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="145" t="s">
+      <c r="A21" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="145"/>
-      <c r="C21" s="145"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="145"/>
-      <c r="F21" s="145"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="145"/>
+      <c r="B21" s="154"/>
+      <c r="C21" s="154"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="154"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="145" t="s">
+      <c r="J21" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="145"/>
-      <c r="L21" s="145"/>
-      <c r="M21" s="145"/>
-      <c r="N21" s="145"/>
-      <c r="O21" s="145"/>
-      <c r="P21" s="145"/>
+      <c r="K21" s="154"/>
+      <c r="L21" s="154"/>
+      <c r="M21" s="154"/>
+      <c r="N21" s="154"/>
+      <c r="O21" s="154"/>
+      <c r="P21" s="154"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="145" t="s">
+      <c r="R21" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="145"/>
-      <c r="T21" s="145"/>
-      <c r="U21" s="145"/>
-      <c r="V21" s="145"/>
-      <c r="W21" s="145"/>
-      <c r="X21" s="145"/>
+      <c r="S21" s="154"/>
+      <c r="T21" s="154"/>
+      <c r="U21" s="154"/>
+      <c r="V21" s="154"/>
+      <c r="W21" s="154"/>
+      <c r="X21" s="154"/>
     </row>
     <row r="23" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="142" t="s">
+      <c r="P23" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="142"/>
-      <c r="R23" s="142"/>
-      <c r="S23" s="142"/>
-      <c r="T23" s="142"/>
-      <c r="U23" s="143" t="s">
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="143"/>
-      <c r="W23" s="143"/>
-      <c r="X23" s="143"/>
+      <c r="V23" s="152"/>
+      <c r="W23" s="152"/>
+      <c r="X23" s="152"/>
     </row>
     <row r="24" spans="1:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="142" t="s">
+      <c r="P24" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="Q24" s="142"/>
-      <c r="R24" s="142"/>
-      <c r="S24" s="142"/>
-      <c r="T24" s="142"/>
-      <c r="U24" s="144" t="s">
+      <c r="Q24" s="151"/>
+      <c r="R24" s="151"/>
+      <c r="S24" s="151"/>
+      <c r="T24" s="151"/>
+      <c r="U24" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="144"/>
-      <c r="W24" s="144"/>
-      <c r="X24" s="144"/>
+      <c r="V24" s="153"/>
+      <c r="W24" s="153"/>
+      <c r="X24" s="153"/>
     </row>
   </sheetData>
   <mergeCells count="40">

</xml_diff>

<commit_message>
feat(Ver. 1.6.1.0): 📚 Stocket - docs:
Se ha actualizado en formato de bitácoras
</commit_message>
<xml_diff>
--- a/docs/GFPI-F-147_Formato_bitácora_etapa_productiva - V2.xlsx
+++ b/docs/GFPI-F-147_Formato_bitácora_etapa_productiva - V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Stocket\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D471B5-3A94-4904-9DBC-9185C900F51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E11D5-64BC-476E-8A3B-C93E3974AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1824,8 +1824,8 @@
   </sheetPr>
   <dimension ref="B1:Y56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
       <c r="N10" s="42"/>
       <c r="O10" s="42"/>
       <c r="P10" s="38">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q10" s="39"/>
       <c r="R10" s="39"/>
@@ -3215,7 +3215,7 @@
     <hyperlink ref="T20" r:id="rId2" xr:uid="{BD6EC083-FDE4-4F22-8CFB-FF65C888314D}"/>
   </hyperlinks>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="60" orientation="portrait" horizontalDpi="4294967294" r:id="rId3"/>
+  <pageSetup scale="59" orientation="portrait" horizontalDpi="4294967294" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>

</xml_diff>